<commit_message>
update mock data to include instructor utorid
</commit_message>
<xml_diff>
--- a/db/seeds/ddah_data.xla.xlsx
+++ b/db/seeds/ddah_data.xla.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t xml:space="preserve">supervisor_utorid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zaleskim</t>
   </si>
   <si>
     <t xml:space="preserve">course_name</t>
@@ -269,38 +272,50 @@
   <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q17" activeCellId="0" sqref="Q17"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="30" min="8" style="0" width="2.42857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.969387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.18877551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.24489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.0357142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="30" min="18" style="0" width="2.29591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>110</v>
@@ -308,92 +323,92 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>5</v>
@@ -401,7 +416,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>6</v>
@@ -409,36 +424,36 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>60</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>10</v>
@@ -476,46 +491,46 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,7 +539,7 @@
         <v>60.00</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>3</v>
@@ -562,7 +577,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>15</v>
@@ -600,7 +615,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">(G14*G17)/60</f>

</xml_diff>

<commit_message>
finish csv ddah importer
</commit_message>
<xml_diff>
--- a/db/seeds/ddah_data.xla.xlsx
+++ b/db/seeds/ddah_data.xla.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">duties_list</t>
   </si>
   <si>
-    <t xml:space="preserve">traingings_list</t>
+    <t xml:space="preserve">trainings_list</t>
   </si>
   <si>
     <t xml:space="preserve">categories_list</t>
@@ -278,30 +278,30 @@
   <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q16" activeCellId="0" sqref="Q16"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="30" min="18" style="0" width="2.02551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="30" min="18" style="0" width="1.88775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>